<commit_message>
change immunity start names to be the same across scenarios
</commit_message>
<xml_diff>
--- a/sensitivity analysis/outputs/S1/S1_start_immunity.xlsx
+++ b/sensitivity analysis/outputs/S1/S1_start_immunity.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,22 +377,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>overall_cdc_indep</t>
+          <t>immunity_all</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>infection_cdc_indep</t>
+          <t>immunity_by_infection</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>vaccination_cdc_indep</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>scenario</t>
+          <t>immunity_by_vaccination</t>
         </is>
       </c>
     </row>
@@ -409,15 +404,10 @@
         <v>70.02730944317058</v>
       </c>
       <c r="D2">
-        <v>25.88631387632144</v>
+        <v>46.34223996473268</v>
       </c>
       <c r="E2">
-        <v>23.68506947843791</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>44.14099556684915</v>
       </c>
     </row>
     <row r="3">
@@ -433,15 +423,10 @@
         <v>64.86236880034181</v>
       </c>
       <c r="D3">
-        <v>31.61292624752544</v>
+        <v>47.35979362050896</v>
       </c>
       <c r="E3">
-        <v>17.50257517983286</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.24944255281638</v>
       </c>
     </row>
     <row r="4">
@@ -457,15 +442,10 @@
         <v>68.07429839972362</v>
       </c>
       <c r="D4">
-        <v>20.77947584661061</v>
+        <v>39.42587209302326</v>
       </c>
       <c r="E4">
-        <v>28.64842630670036</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>47.294822553113</v>
       </c>
     </row>
     <row r="5">
@@ -481,15 +461,10 @@
         <v>60.73960953329535</v>
       </c>
       <c r="D5">
-        <v>28.60454382469332</v>
+        <v>42.14922496185045</v>
       </c>
       <c r="E5">
-        <v>18.5903845714449</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>32.13506570860204</v>
       </c>
     </row>
     <row r="6">
@@ -505,15 +480,10 @@
         <v>62.96434089255383</v>
       </c>
       <c r="D6">
-        <v>18.58512194042807</v>
+        <v>33.41398950228939</v>
       </c>
       <c r="E6">
-        <v>29.55035139026442</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>44.37921895212575</v>
       </c>
     </row>
     <row r="7">
@@ -529,15 +499,10 @@
         <v>71.20155585106799</v>
       </c>
       <c r="D7">
-        <v>28.09001932107519</v>
+        <v>49.37735633497087</v>
       </c>
       <c r="E7">
-        <v>21.82419951609712</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>43.1115365299928</v>
       </c>
     </row>
     <row r="8">
@@ -553,15 +518,10 @@
         <v>65.58625192603046</v>
       </c>
       <c r="D8">
-        <v>23.22109318270547</v>
+        <v>40.29002713704206</v>
       </c>
       <c r="E8">
-        <v>25.29622478898841</v>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>42.365158743325</v>
       </c>
     </row>
     <row r="9">
@@ -577,15 +537,10 @@
         <v>62.51198290116067</v>
       </c>
       <c r="D9">
-        <v>22.10169512028028</v>
+        <v>37.08978328173374</v>
       </c>
       <c r="E9">
-        <v>25.42219961942692</v>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>40.41028778088039</v>
       </c>
     </row>
     <row r="10">
@@ -601,15 +556,10 @@
         <v>57.922251906596</v>
       </c>
       <c r="D10">
-        <v>27.36311198446723</v>
+        <v>39.40491513754603</v>
       </c>
       <c r="E10">
-        <v>18.51733676904998</v>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>30.55913992212878</v>
       </c>
     </row>
     <row r="11">
@@ -625,15 +575,10 @@
         <v>67.10336400731262</v>
       </c>
       <c r="D11">
-        <v>12.91467955721582</v>
+        <v>28.1910253006107</v>
       </c>
       <c r="E11">
-        <v>38.91233870670192</v>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>54.18868445009682</v>
       </c>
     </row>
     <row r="12">
@@ -649,15 +594,10 @@
         <v>65.39572517258475</v>
       </c>
       <c r="D12">
-        <v>13.46967327336564</v>
+        <v>28.0186541890177</v>
       </c>
       <c r="E12">
-        <v>37.37707098356705</v>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>51.9260518992191</v>
       </c>
     </row>
     <row r="13">
@@ -673,15 +613,10 @@
         <v>64.30190483965585</v>
       </c>
       <c r="D13">
-        <v>28.938964600279</v>
+        <v>44.77147430197404</v>
       </c>
       <c r="E13">
-        <v>19.53043053768181</v>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.36294023937685</v>
       </c>
     </row>
     <row r="14">
@@ -697,15 +632,10 @@
         <v>65.51978999257489</v>
       </c>
       <c r="D14">
-        <v>25.85745623309237</v>
+        <v>42.8545846138954</v>
       </c>
       <c r="E14">
-        <v>22.66520537867948</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.66233375948252</v>
       </c>
     </row>
     <row r="15">
@@ -721,15 +651,10 @@
         <v>65.69019653334472</v>
       </c>
       <c r="D15">
-        <v>29.68035567746827</v>
+        <v>46.38268770455767</v>
       </c>
       <c r="E15">
-        <v>19.30750882878706</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.00984085587645</v>
       </c>
     </row>
     <row r="16">
@@ -745,15 +670,10 @@
         <v>49.74616561080042</v>
       </c>
       <c r="D16">
-        <v>17.9427195195393</v>
+        <v>26.31030234101033</v>
       </c>
       <c r="E16">
-        <v>23.43586326979008</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>31.80344609126111</v>
       </c>
     </row>
     <row r="17">
@@ -769,15 +689,10 @@
         <v>61.83769522769903</v>
       </c>
       <c r="D17">
-        <v>16.73107668096297</v>
+        <v>30.47922397567685</v>
       </c>
       <c r="E17">
-        <v>31.35847125202218</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>45.10661854673607</v>
       </c>
     </row>
     <row r="18">
@@ -793,15 +708,10 @@
         <v>60.16679534207324</v>
       </c>
       <c r="D18">
-        <v>24.80030138359044</v>
+        <v>38.37065773232234</v>
       </c>
       <c r="E18">
-        <v>21.79613760975091</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.36649395848281</v>
       </c>
     </row>
     <row r="19">
@@ -817,15 +727,10 @@
         <v>70.02999947730115</v>
       </c>
       <c r="D19">
-        <v>30.03205336595322</v>
+        <v>50.0517089326388</v>
       </c>
       <c r="E19">
-        <v>19.97829054466234</v>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.99794611134792</v>
       </c>
     </row>
     <row r="20">
@@ -841,15 +746,10 @@
         <v>62.35678329706501</v>
       </c>
       <c r="D20">
-        <v>13.58321100211206</v>
+        <v>26.51602231629707</v>
       </c>
       <c r="E20">
-        <v>35.84076098076795</v>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>48.77357229495296</v>
       </c>
     </row>
     <row r="21">
@@ -865,15 +765,10 @@
         <v>58.31850118538099</v>
       </c>
       <c r="D21">
-        <v>24.6432346635672</v>
+        <v>37.15542207443956</v>
       </c>
       <c r="E21">
-        <v>21.16307911094144</v>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.6752665218138</v>
       </c>
     </row>
     <row r="22">
@@ -889,15 +784,10 @@
         <v>66.64763172635948</v>
       </c>
       <c r="D22">
-        <v>24.20282031168331</v>
+        <v>42.05150031921686</v>
       </c>
       <c r="E22">
-        <v>24.59613140714263</v>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>42.44481141467617</v>
       </c>
     </row>
     <row r="23">
@@ -913,15 +803,10 @@
         <v>56.13543392163417</v>
       </c>
       <c r="D23">
-        <v>21.81827117112697</v>
+        <v>33.21761374017906</v>
       </c>
       <c r="E23">
-        <v>22.91782018145513</v>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>34.31716275050722</v>
       </c>
     </row>
     <row r="24">
@@ -937,15 +822,10 @@
         <v>65.57507377904605</v>
       </c>
       <c r="D24">
-        <v>31.39774119181468</v>
+        <v>47.70049957854485</v>
       </c>
       <c r="E24">
-        <v>17.87457420050121</v>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>34.17733258723138</v>
       </c>
     </row>
     <row r="25">
@@ -961,15 +841,10 @@
         <v>62.3202043954489</v>
       </c>
       <c r="D25">
-        <v>31.47794892720127</v>
+        <v>45.51615894984661</v>
       </c>
       <c r="E25">
-        <v>16.80404544560228</v>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>30.84225546824763</v>
       </c>
     </row>
     <row r="26">
@@ -985,15 +860,10 @@
         <v>61.18667326976369</v>
       </c>
       <c r="D26">
-        <v>22.5919288137899</v>
+        <v>36.79152315813096</v>
       </c>
       <c r="E26">
-        <v>24.39515011163272</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.59474445597377</v>
       </c>
     </row>
     <row r="27">
@@ -1009,15 +879,10 @@
         <v>52.96257530991479</v>
       </c>
       <c r="D27">
-        <v>26.55598453753256</v>
+        <v>36.08473206533658</v>
       </c>
       <c r="E27">
-        <v>16.87784324457821</v>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>26.40659077238223</v>
       </c>
     </row>
     <row r="28">
@@ -1033,15 +898,10 @@
         <v>50.90415590077034</v>
       </c>
       <c r="D28">
-        <v>15.42949305556327</v>
+        <v>23.91230133141145</v>
       </c>
       <c r="E28">
-        <v>26.9918545693589</v>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.47466284520707</v>
       </c>
     </row>
     <row r="29">
@@ -1057,15 +917,10 @@
         <v>71.09556966815306</v>
       </c>
       <c r="D29">
-        <v>9.092821445759212</v>
+        <v>23.93020816078626</v>
       </c>
       <c r="E29">
-        <v>47.1653615073668</v>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>62.00274822239385</v>
       </c>
     </row>
     <row r="30">
@@ -1081,15 +936,10 @@
         <v>61.37752493727723</v>
       </c>
       <c r="D30">
-        <v>26.89426509655179</v>
+        <v>41.04945549972488</v>
       </c>
       <c r="E30">
-        <v>20.32806943755235</v>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>34.48325984072544</v>
       </c>
     </row>
     <row r="31">
@@ -1105,15 +955,10 @@
         <v>66.03362059647712</v>
       </c>
       <c r="D31">
-        <v>22.15112047741179</v>
+        <v>39.47275007691034</v>
       </c>
       <c r="E31">
-        <v>26.5608705195668</v>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>43.88250011906534</v>
       </c>
     </row>
     <row r="32">
@@ -1129,15 +974,10 @@
         <v>58.93835238541774</v>
       </c>
       <c r="D32">
-        <v>30.72045712257561</v>
+        <v>42.7968185595333</v>
       </c>
       <c r="E32">
-        <v>16.14153382588444</v>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>28.21789526284213</v>
       </c>
     </row>
     <row r="33">
@@ -1153,15 +993,10 @@
         <v>69.70715264694971</v>
       </c>
       <c r="D33">
-        <v>14.83011956145909</v>
+        <v>32.86601164669968</v>
       </c>
       <c r="E33">
-        <v>36.84114100025003</v>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>54.87703308549062</v>
       </c>
     </row>
     <row r="34">
@@ -1177,15 +1012,10 @@
         <v>62.08616063243743</v>
       </c>
       <c r="D34">
-        <v>28.83602068538801</v>
+        <v>43.20012156207264</v>
       </c>
       <c r="E34">
-        <v>18.8860390703648</v>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.25013994704943</v>
       </c>
     </row>
     <row r="35">
@@ -1201,15 +1031,10 @@
         <v>68.57354286436373</v>
       </c>
       <c r="D35">
-        <v>20.4198802401131</v>
+        <v>39.38538626580845</v>
       </c>
       <c r="E35">
-        <v>29.1881565985553</v>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>48.15366262425064</v>
       </c>
     </row>
     <row r="36">
@@ -1225,15 +1050,10 @@
         <v>65.65245273370448</v>
       </c>
       <c r="D36">
-        <v>25.00800535299262</v>
+        <v>42.1325457340044</v>
       </c>
       <c r="E36">
-        <v>23.51990699970007</v>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>40.64444738071186</v>
       </c>
     </row>
     <row r="37">
@@ -1249,15 +1069,10 @@
         <v>67.93885497819821</v>
       </c>
       <c r="D37">
-        <v>31.27575601045642</v>
+        <v>49.37999097007813</v>
       </c>
       <c r="E37">
-        <v>18.55886400812008</v>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.66309896774178</v>
       </c>
     </row>
     <row r="38">
@@ -1273,15 +1088,10 @@
         <v>48.74567411806898</v>
       </c>
       <c r="D38">
-        <v>17.79431565849589</v>
+        <v>25.77069622445445</v>
       </c>
       <c r="E38">
-        <v>22.97497789361452</v>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>30.95135845957309</v>
       </c>
     </row>
     <row r="39">
@@ -1297,15 +1107,10 @@
         <v>52.66426537443039</v>
       </c>
       <c r="D39">
-        <v>21.76355614968718</v>
+        <v>31.49606299212599</v>
       </c>
       <c r="E39">
-        <v>21.1682023823044</v>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>30.90070922474321</v>
       </c>
     </row>
     <row r="40">
@@ -1321,15 +1126,10 @@
         <v>65.6074085002231</v>
       </c>
       <c r="D40">
-        <v>23.12357910848682</v>
+        <v>40.20361380798274</v>
       </c>
       <c r="E40">
-        <v>25.40379469224036</v>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>42.48382939173629</v>
       </c>
     </row>
     <row r="41">
@@ -1345,15 +1145,10 @@
         <v>67.65994332921551</v>
       </c>
       <c r="D41">
-        <v>27.55326127907992</v>
+        <v>46.00389863547758</v>
       </c>
       <c r="E41">
-        <v>21.65604469373794</v>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>40.1066820501356</v>
       </c>
     </row>
     <row r="42">
@@ -1369,15 +1164,10 @@
         <v>66.56315018990746</v>
       </c>
       <c r="D42">
-        <v>19.4950355453827</v>
+        <v>36.83041972614366</v>
       </c>
       <c r="E42">
-        <v>29.7327304637638</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>47.06811464452477</v>
       </c>
     </row>
     <row r="43">
@@ -1393,15 +1183,10 @@
         <v>65.53578517380656</v>
       </c>
       <c r="D43">
-        <v>27.29532998066935</v>
+        <v>44.19613205704239</v>
       </c>
       <c r="E43">
-        <v>21.33965311676416</v>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.24045519313722</v>
       </c>
     </row>
     <row r="44">
@@ -1417,15 +1202,10 @@
         <v>54.51914533861141</v>
       </c>
       <c r="D44">
-        <v>25.78679713705094</v>
+        <v>36.18303183326655</v>
       </c>
       <c r="E44">
-        <v>18.33611350534486</v>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>28.73234820156047</v>
       </c>
     </row>
     <row r="45">
@@ -1441,15 +1221,10 @@
         <v>61.47892229246585</v>
       </c>
       <c r="D45">
-        <v>16.00393463285679</v>
+        <v>29.35154701652662</v>
       </c>
       <c r="E45">
-        <v>32.12737527593922</v>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>45.47498765960906</v>
       </c>
     </row>
     <row r="46">
@@ -1465,15 +1240,10 @@
         <v>65.17286589395687</v>
       </c>
       <c r="D46">
-        <v>19.29832350918705</v>
+        <v>35.65479971804756</v>
       </c>
       <c r="E46">
-        <v>29.51806617590932</v>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>45.87454238476984</v>
       </c>
     </row>
     <row r="47">
@@ -1489,15 +1259,10 @@
         <v>57.12344253814953</v>
       </c>
       <c r="D47">
-        <v>23.13728568856973</v>
+        <v>35.04914209561885</v>
       </c>
       <c r="E47">
-        <v>22.07430044253067</v>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.98615684957979</v>
       </c>
     </row>
     <row r="48">
@@ -1513,15 +1278,10 @@
         <v>49.67063185293076</v>
       </c>
       <c r="D48">
-        <v>28.41854303493496</v>
+        <v>36.08799599681227</v>
       </c>
       <c r="E48">
-        <v>13.58263585611849</v>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>21.25208881799581</v>
       </c>
     </row>
     <row r="49">
@@ -1537,15 +1297,10 @@
         <v>77.03503264196948</v>
       </c>
       <c r="D49">
-        <v>24.22319773357892</v>
+        <v>51.33320544791866</v>
       </c>
       <c r="E49">
-        <v>25.70182719405081</v>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>52.81183490839057</v>
       </c>
     </row>
     <row r="50">
@@ -1561,15 +1316,10 @@
         <v>65.32528900875121</v>
       </c>
       <c r="D50">
-        <v>26.91316129431056</v>
+        <v>43.69880025977281</v>
       </c>
       <c r="E50">
-        <v>21.62648874897839</v>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.41212771444065</v>
       </c>
     </row>
     <row r="51">
@@ -1585,15 +1335,10 @@
         <v>60.12046682185805</v>
       </c>
       <c r="D51">
-        <v>20.48665858675473</v>
+        <v>33.93730495132517</v>
       </c>
       <c r="E51">
-        <v>26.18316187053288</v>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.63380823510331</v>
       </c>
     </row>
     <row r="52">
@@ -1609,15 +1354,10 @@
         <v>66.51762707264456</v>
       </c>
       <c r="D52">
-        <v>27.16195664197191</v>
+        <v>44.78894702087672</v>
       </c>
       <c r="E52">
-        <v>21.72868005176783</v>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.35567043067265</v>
       </c>
     </row>
     <row r="53">
@@ -1633,15 +1373,10 @@
         <v>60.54522714514135</v>
       </c>
       <c r="D53">
-        <v>23.82324298758767</v>
+        <v>37.64853033145716</v>
       </c>
       <c r="E53">
-        <v>22.89669681368419</v>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.72198415755368</v>
       </c>
     </row>
     <row r="54">
@@ -1657,15 +1392,10 @@
         <v>63.79736837003704</v>
       </c>
       <c r="D54">
-        <v>24.59683977235815</v>
+        <v>40.4556802962914</v>
       </c>
       <c r="E54">
-        <v>23.34168807374563</v>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.20052859767888</v>
       </c>
     </row>
     <row r="55">
@@ -1681,15 +1411,10 @@
         <v>65.85434349643346</v>
       </c>
       <c r="D55">
-        <v>26.91202719260306</v>
+        <v>44.07639720910564</v>
       </c>
       <c r="E55">
-        <v>21.7779462873278</v>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.9423163038304</v>
       </c>
     </row>
     <row r="56">
@@ -1705,15 +1430,10 @@
         <v>68.72289432090854</v>
       </c>
       <c r="D56">
-        <v>30.47356280836265</v>
+        <v>49.34936504299377</v>
       </c>
       <c r="E56">
-        <v>19.37352927791477</v>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.24933151254588</v>
       </c>
     </row>
     <row r="57">
@@ -1729,15 +1449,10 @@
         <v>67.03704153074085</v>
       </c>
       <c r="D57">
-        <v>18.65128491626322</v>
+        <v>36.13592623445265</v>
       </c>
       <c r="E57">
-        <v>30.90111529628821</v>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>48.38575661447764</v>
       </c>
     </row>
     <row r="58">
@@ -1753,15 +1468,10 @@
         <v>62.3449247555107</v>
       </c>
       <c r="D58">
-        <v>15.83329361453122</v>
+        <v>29.60137680822364</v>
       </c>
       <c r="E58">
-        <v>32.74354794728706</v>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>46.51163114097948</v>
       </c>
     </row>
     <row r="59">
@@ -1777,15 +1487,10 @@
         <v>59.8782003576008</v>
       </c>
       <c r="D59">
-        <v>25.97835177653362</v>
+        <v>39.30150115978817</v>
       </c>
       <c r="E59">
-        <v>20.57669919781262</v>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.89984858106718</v>
       </c>
     </row>
     <row r="60">
@@ -1801,15 +1506,10 @@
         <v>66.33836358202474</v>
       </c>
       <c r="D60">
-        <v>28.83743293116743</v>
+        <v>46.1405797421894</v>
       </c>
       <c r="E60">
-        <v>20.19778383983535</v>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>37.50093065085732</v>
       </c>
     </row>
     <row r="61">
@@ -1825,15 +1525,10 @@
         <v>69.86255754671389</v>
       </c>
       <c r="D61">
-        <v>22.21958026196167</v>
+        <v>42.43858628632588</v>
       </c>
       <c r="E61">
-        <v>27.42397126038802</v>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>47.64297728475222</v>
       </c>
     </row>
     <row r="62">
@@ -1849,15 +1544,10 @@
         <v>61.5308675634152</v>
       </c>
       <c r="D62">
-        <v>24.62562741021432</v>
+        <v>39.02959210877099</v>
       </c>
       <c r="E62">
-        <v>22.5012754546442</v>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.90524015320087</v>
       </c>
     </row>
     <row r="63">
@@ -1873,15 +1563,10 @@
         <v>66.25539316288834</v>
       </c>
       <c r="D63">
-        <v>33.06794950733521</v>
+        <v>49.49361514751211</v>
       </c>
       <c r="E63">
-        <v>16.76177801537624</v>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.18744365555313</v>
       </c>
     </row>
     <row r="64">
@@ -1897,15 +1582,10 @@
         <v>65.54369331309398</v>
       </c>
       <c r="D64">
-        <v>20.14113155282288</v>
+        <v>36.89025016958908</v>
       </c>
       <c r="E64">
-        <v>28.6534431435049</v>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>45.40256176027109</v>
       </c>
     </row>
     <row r="65">
@@ -1921,15 +1601,10 @@
         <v>71.02252475236101</v>
       </c>
       <c r="D65">
-        <v>28.34469409505243</v>
+        <v>49.44804849516112</v>
       </c>
       <c r="E65">
-        <v>21.57447625719989</v>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>42.67783065730858</v>
       </c>
     </row>
     <row r="66">
@@ -1945,15 +1620,10 @@
         <v>67.86866725775438</v>
       </c>
       <c r="D66">
-        <v>16.66053249033657</v>
+        <v>34.14612745571164</v>
       </c>
       <c r="E66">
-        <v>33.72253980204273</v>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>51.2081347674178</v>
       </c>
     </row>
     <row r="67">
@@ -1969,15 +1639,10 @@
         <v>60.36348825931987</v>
       </c>
       <c r="D67">
-        <v>24.02831860072798</v>
+        <v>37.74190313847388</v>
       </c>
       <c r="E67">
-        <v>22.62158512084599</v>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.33516965859189</v>
       </c>
     </row>
     <row r="68">
@@ -1993,15 +1658,10 @@
         <v>50.99693440994652</v>
       </c>
       <c r="D68">
-        <v>28.17447788012699</v>
+        <v>36.50605683117256</v>
       </c>
       <c r="E68">
-        <v>14.49087757877396</v>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>22.82245652981953</v>
       </c>
     </row>
     <row r="69">
@@ -2017,15 +1677,10 @@
         <v>71.92948512553262</v>
       </c>
       <c r="D69">
-        <v>8.67455121459626</v>
+        <v>23.60739042779419</v>
       </c>
       <c r="E69">
-        <v>48.32209469773844</v>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>63.25493391093637</v>
       </c>
     </row>
     <row r="70">
@@ -2041,15 +1696,10 @@
         <v>62.54919858471973</v>
       </c>
       <c r="D70">
-        <v>20.0727962114551</v>
+        <v>34.89489016612865</v>
       </c>
       <c r="E70">
-        <v>27.65430841859107</v>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>42.47640237326462</v>
       </c>
     </row>
     <row r="71">
@@ -2065,15 +1715,10 @@
         <v>60.08643524549549</v>
       </c>
       <c r="D71">
-        <v>21.22080991444235</v>
+        <v>34.71174773498001</v>
       </c>
       <c r="E71">
-        <v>25.37468751051549</v>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.86562533105315</v>
       </c>
     </row>
     <row r="72">
@@ -2089,15 +1734,10 @@
         <v>61.32983269544311</v>
       </c>
       <c r="D72">
-        <v>22.27598605055445</v>
+        <v>36.55027401115913</v>
       </c>
       <c r="E72">
-        <v>24.77955868428398</v>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.05384664488866</v>
       </c>
     </row>
     <row r="73">
@@ -2113,15 +1753,10 @@
         <v>55.3897829452142</v>
       </c>
       <c r="D73">
-        <v>19.90789785430027</v>
+        <v>30.85629188384215</v>
       </c>
       <c r="E73">
-        <v>24.53349106137205</v>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.48188509091392</v>
       </c>
     </row>
     <row r="74">
@@ -2137,15 +1772,10 @@
         <v>61.62477907578864</v>
       </c>
       <c r="D74">
-        <v>20.95414633041932</v>
+        <v>35.3183377811666</v>
       </c>
       <c r="E74">
-        <v>26.30644129462203</v>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>40.67063274536932</v>
       </c>
     </row>
     <row r="75">
@@ -2161,15 +1791,10 @@
         <v>68.04455619720748</v>
       </c>
       <c r="D75">
-        <v>27.02592332208908</v>
+        <v>45.8211205326369</v>
       </c>
       <c r="E75">
-        <v>22.22343566457057</v>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>41.01863287511839</v>
       </c>
     </row>
     <row r="76">
@@ -2185,15 +1810,10 @@
         <v>56.24809844603809</v>
       </c>
       <c r="D76">
-        <v>17.98245497323934</v>
+        <v>29.12876392469718</v>
       </c>
       <c r="E76">
-        <v>27.11933452134091</v>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.26564347279876</v>
       </c>
     </row>
     <row r="77">
@@ -2209,15 +1829,10 @@
         <v>60.76669004226036</v>
       </c>
       <c r="D77">
-        <v>29.28733601072474</v>
+        <v>42.74235246440001</v>
       </c>
       <c r="E77">
-        <v>18.02433757786036</v>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>31.47935403153563</v>
       </c>
     </row>
     <row r="78">
@@ -2233,15 +1848,10 @@
         <v>61.52653017942522</v>
       </c>
       <c r="D78">
-        <v>28.28281450890515</v>
+        <v>42.36726892903972</v>
       </c>
       <c r="E78">
-        <v>19.15926125038552</v>
-      </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.24371567052008</v>
       </c>
     </row>
     <row r="79">
@@ -2257,15 +1867,10 @@
         <v>62.19427610829506</v>
       </c>
       <c r="D79">
-        <v>37.94054031416552</v>
+        <v>50.08899212645932</v>
       </c>
       <c r="E79">
-        <v>12.10528398183576</v>
-      </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>24.25373579412955</v>
       </c>
     </row>
     <row r="80">
@@ -2281,15 +1886,10 @@
         <v>59.80810706157654</v>
       </c>
       <c r="D80">
-        <v>22.45776790042015</v>
+        <v>35.84659134578433</v>
       </c>
       <c r="E80">
-        <v>23.9615157157922</v>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>37.35033916115638</v>
       </c>
     </row>
     <row r="81">
@@ -2305,15 +1905,10 @@
         <v>63.73825614232677</v>
       </c>
       <c r="D81">
-        <v>34.36488897573585</v>
+        <v>48.65712493584991</v>
       </c>
       <c r="E81">
-        <v>15.08113120647685</v>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>29.37336716659092</v>
       </c>
     </row>
     <row r="82">
@@ -2329,15 +1924,10 @@
         <v>61.30019752350766</v>
       </c>
       <c r="D82">
-        <v>31.19492688301719</v>
+        <v>44.63130077028183</v>
       </c>
       <c r="E82">
-        <v>16.66889675322581</v>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>30.10527064049046</v>
       </c>
     </row>
     <row r="83">
@@ -2353,15 +1943,10 @@
         <v>67.7225646049325</v>
       </c>
       <c r="D83">
-        <v>33.49672446721682</v>
+        <v>50.92687544371697</v>
       </c>
       <c r="E83">
-        <v>16.79568916121552</v>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>34.22584013771567</v>
       </c>
     </row>
     <row r="84">
@@ -2377,15 +1962,10 @@
         <v>64.15211341183061</v>
       </c>
       <c r="D84">
-        <v>28.50218864041963</v>
+        <v>44.29239365948226</v>
       </c>
       <c r="E84">
-        <v>19.85971975234835</v>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.64992477141099</v>
       </c>
     </row>
     <row r="85">
@@ -2401,15 +1981,10 @@
         <v>66.92864884445585</v>
       </c>
       <c r="D85">
-        <v>34.91257324257511</v>
+        <v>51.35415990127947</v>
       </c>
       <c r="E85">
-        <v>15.57448894317637</v>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>32.01607560188073</v>
       </c>
     </row>
     <row r="86">
@@ -2425,15 +2000,10 @@
         <v>59.15437932249601</v>
       </c>
       <c r="D86">
-        <v>23.90121496658071</v>
+        <v>36.91487735086609</v>
       </c>
       <c r="E86">
-        <v>22.23950197162992</v>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.2531643559153</v>
       </c>
     </row>
     <row r="87">
@@ -2449,15 +2019,10 @@
         <v>66.80739304646269</v>
       </c>
       <c r="D87">
-        <v>28.89074019823467</v>
+        <v>46.53541009573301</v>
       </c>
       <c r="E87">
-        <v>20.27198295072969</v>
-      </c>
-      <c r="F87" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>37.91665284822803</v>
       </c>
     </row>
     <row r="88">
@@ -2473,15 +2038,10 @@
         <v>53.62995100287824</v>
       </c>
       <c r="D88">
-        <v>23.67623264471682</v>
+        <v>33.80084151472651</v>
       </c>
       <c r="E88">
-        <v>19.82910948815174</v>
-      </c>
-      <c r="F88" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>29.95371835816143</v>
       </c>
     </row>
     <row r="89">
@@ -2497,15 +2057,10 @@
         <v>62.66304346344287</v>
       </c>
       <c r="D89">
-        <v>14.58611782512678</v>
+        <v>28.09178386380459</v>
       </c>
       <c r="E89">
-        <v>34.57125959963828</v>
-      </c>
-      <c r="F89" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>48.07692563831609</v>
       </c>
     </row>
     <row r="90">
@@ -2521,15 +2076,10 @@
         <v>54.69587295496076</v>
       </c>
       <c r="D90">
-        <v>20.88224478850899</v>
+        <v>31.55067155067155</v>
       </c>
       <c r="E90">
-        <v>23.14520140428921</v>
-      </c>
-      <c r="F90" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.81362816645177</v>
       </c>
     </row>
     <row r="91">
@@ -2545,15 +2095,10 @@
         <v>65.48601935897834</v>
       </c>
       <c r="D91">
-        <v>25.70909320183824</v>
+        <v>42.6897724764448</v>
       </c>
       <c r="E91">
-        <v>22.79624688253353</v>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>39.77692615714009</v>
       </c>
     </row>
     <row r="92">
@@ -2569,15 +2114,10 @@
         <v>67.0834668484257</v>
       </c>
       <c r="D92">
-        <v>26.63097073457989</v>
+        <v>44.72222846736662</v>
       </c>
       <c r="E92">
-        <v>22.36123838105908</v>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>40.45249611384582</v>
       </c>
     </row>
     <row r="93">
@@ -2593,15 +2133,10 @@
         <v>72.40363024616074</v>
       </c>
       <c r="D93">
-        <v>13.84402177295858</v>
+        <v>33.40707281688257</v>
       </c>
       <c r="E93">
-        <v>38.99655742927818</v>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>58.55960847320218</v>
       </c>
     </row>
     <row r="94">
@@ -2617,15 +2152,10 @@
         <v>62.76961228782721</v>
       </c>
       <c r="D94">
-        <v>21.36874649893416</v>
+        <v>36.46597648004825</v>
       </c>
       <c r="E94">
-        <v>26.30363580777898</v>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>41.40086578889306</v>
       </c>
     </row>
     <row r="95">
@@ -2641,15 +2171,10 @@
         <v>61.10512371470648</v>
       </c>
       <c r="D95">
-        <v>24.26294380095946</v>
+        <v>38.41637309176313</v>
       </c>
       <c r="E95">
-        <v>22.68875062294336</v>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>36.84217991374702</v>
       </c>
     </row>
     <row r="96">
@@ -2665,15 +2190,10 @@
         <v>70.60175595229825</v>
       </c>
       <c r="D96">
-        <v>17.02114805579166</v>
+        <v>36.6681838871188</v>
       </c>
       <c r="E96">
-        <v>33.93357206517945</v>
-      </c>
-      <c r="F96" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>53.58060789650659</v>
       </c>
     </row>
     <row r="97">
@@ -2689,15 +2209,10 @@
         <v>55.9176249931736</v>
       </c>
       <c r="D97">
-        <v>26.17737403533636</v>
+        <v>37.25799535609977</v>
       </c>
       <c r="E97">
-        <v>18.65962963707382</v>
-      </c>
-      <c r="F97" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>29.74025095783723</v>
       </c>
     </row>
     <row r="98">
@@ -2713,15 +2228,10 @@
         <v>60.13558656378957</v>
       </c>
       <c r="D98">
-        <v>27.1051015811827</v>
+        <v>40.47379105872731</v>
       </c>
       <c r="E98">
-        <v>19.66179550506227</v>
-      </c>
-      <c r="F98" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>33.03048498260687</v>
       </c>
     </row>
     <row r="99">
@@ -2737,15 +2247,10 @@
         <v>66.45624943864954</v>
       </c>
       <c r="D99">
-        <v>31.17007585744027</v>
+        <v>48.16602198072082</v>
       </c>
       <c r="E99">
-        <v>18.2902274579287</v>
-      </c>
-      <c r="F99" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.28617358120925</v>
       </c>
     </row>
     <row r="100">
@@ -2761,15 +2266,10 @@
         <v>63.9443222281895</v>
       </c>
       <c r="D100">
-        <v>28.20470688908716</v>
+        <v>43.89128237859688</v>
       </c>
       <c r="E100">
-        <v>20.05303984959261</v>
-      </c>
-      <c r="F100" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>35.73961533910233</v>
       </c>
     </row>
     <row r="101">
@@ -2785,15 +2285,10 @@
         <v>61.17697701880255</v>
       </c>
       <c r="D101">
-        <v>22.38941382154285</v>
+        <v>36.57657657657658</v>
       </c>
       <c r="E101">
-        <v>24.60040044222596</v>
-      </c>
-      <c r="F101" t="inlineStr">
-        <is>
-          <t>S1</t>
-        </is>
+        <v>38.78756319725969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
push all NEW maps S1-6, should be corrected, I double/triple checked
</commit_message>
<xml_diff>
--- a/sensitivity analysis/outputs/S1/S1_start_immunity.xlsx
+++ b/sensitivity analysis/outputs/S1/S1_start_immunity.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -390,6 +390,11 @@
           <t>immunity_by_vaccination</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>scenario</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -409,6 +414,11 @@
       <c r="E2">
         <v>44.14099556684915</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -428,6 +438,11 @@
       <c r="E3">
         <v>33.24944255281638</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -447,6 +462,11 @@
       <c r="E4">
         <v>47.294822553113</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -466,6 +486,11 @@
       <c r="E5">
         <v>32.13506570860204</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -485,6 +510,11 @@
       <c r="E6">
         <v>44.37921895212575</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -504,6 +534,11 @@
       <c r="E7">
         <v>43.1115365299928</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -523,6 +558,11 @@
       <c r="E8">
         <v>42.365158743325</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -542,6 +582,11 @@
       <c r="E9">
         <v>40.41028778088039</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -561,6 +606,11 @@
       <c r="E10">
         <v>30.55913992212878</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -580,6 +630,11 @@
       <c r="E11">
         <v>54.18868445009682</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -599,6 +654,11 @@
       <c r="E12">
         <v>51.9260518992191</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -618,6 +678,11 @@
       <c r="E13">
         <v>35.36294023937685</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -637,6 +702,11 @@
       <c r="E14">
         <v>39.66233375948252</v>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -656,6 +726,11 @@
       <c r="E15">
         <v>36.00984085587645</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -675,6 +750,11 @@
       <c r="E16">
         <v>31.80344609126111</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -694,6 +774,11 @@
       <c r="E17">
         <v>45.10661854673607</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -713,6 +798,11 @@
       <c r="E18">
         <v>35.36649395848281</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -732,6 +822,11 @@
       <c r="E19">
         <v>39.99794611134792</v>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -751,6 +846,11 @@
       <c r="E20">
         <v>48.77357229495296</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -770,6 +870,11 @@
       <c r="E21">
         <v>33.6752665218138</v>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -789,6 +894,11 @@
       <c r="E22">
         <v>42.44481141467617</v>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -808,6 +918,11 @@
       <c r="E23">
         <v>34.31716275050722</v>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -827,6 +942,11 @@
       <c r="E24">
         <v>34.17733258723138</v>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -846,6 +966,11 @@
       <c r="E25">
         <v>30.84225546824763</v>
       </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -865,6 +990,11 @@
       <c r="E26">
         <v>38.59474445597377</v>
       </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -884,6 +1014,11 @@
       <c r="E27">
         <v>26.40659077238223</v>
       </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -903,6 +1038,11 @@
       <c r="E28">
         <v>35.47466284520707</v>
       </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -922,6 +1062,11 @@
       <c r="E29">
         <v>62.00274822239385</v>
       </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -941,6 +1086,11 @@
       <c r="E30">
         <v>34.48325984072544</v>
       </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -960,6 +1110,11 @@
       <c r="E31">
         <v>43.88250011906534</v>
       </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -979,6 +1134,11 @@
       <c r="E32">
         <v>28.21789526284213</v>
       </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -998,6 +1158,11 @@
       <c r="E33">
         <v>54.87703308549062</v>
       </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1017,6 +1182,11 @@
       <c r="E34">
         <v>33.25013994704943</v>
       </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1036,6 +1206,11 @@
       <c r="E35">
         <v>48.15366262425064</v>
       </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1055,6 +1230,11 @@
       <c r="E36">
         <v>40.64444738071186</v>
       </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1074,6 +1254,11 @@
       <c r="E37">
         <v>36.66309896774178</v>
       </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1093,6 +1278,11 @@
       <c r="E38">
         <v>30.95135845957309</v>
       </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1112,6 +1302,11 @@
       <c r="E39">
         <v>30.90070922474321</v>
       </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1131,6 +1326,11 @@
       <c r="E40">
         <v>42.48382939173629</v>
       </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1150,6 +1350,11 @@
       <c r="E41">
         <v>40.1066820501356</v>
       </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1169,6 +1374,11 @@
       <c r="E42">
         <v>47.06811464452477</v>
       </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1188,6 +1398,11 @@
       <c r="E43">
         <v>38.24045519313722</v>
       </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1207,6 +1422,11 @@
       <c r="E44">
         <v>28.73234820156047</v>
       </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1226,6 +1446,11 @@
       <c r="E45">
         <v>45.47498765960906</v>
       </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1245,6 +1470,11 @@
       <c r="E46">
         <v>45.87454238476984</v>
       </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1264,6 +1494,11 @@
       <c r="E47">
         <v>33.98615684957979</v>
       </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1283,6 +1518,11 @@
       <c r="E48">
         <v>21.25208881799581</v>
       </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1302,6 +1542,11 @@
       <c r="E49">
         <v>52.81183490839057</v>
       </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1321,6 +1566,11 @@
       <c r="E50">
         <v>38.41212771444065</v>
       </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -1340,6 +1590,11 @@
       <c r="E51">
         <v>39.63380823510331</v>
       </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -1359,6 +1614,11 @@
       <c r="E52">
         <v>39.35567043067265</v>
       </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -1378,6 +1638,11 @@
       <c r="E53">
         <v>36.72198415755368</v>
       </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -1397,6 +1662,11 @@
       <c r="E54">
         <v>39.20052859767888</v>
       </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -1416,6 +1686,11 @@
       <c r="E55">
         <v>38.9423163038304</v>
       </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -1435,6 +1710,11 @@
       <c r="E56">
         <v>38.24933151254588</v>
       </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -1454,6 +1734,11 @@
       <c r="E57">
         <v>48.38575661447764</v>
       </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -1473,6 +1758,11 @@
       <c r="E58">
         <v>46.51163114097948</v>
       </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -1492,6 +1782,11 @@
       <c r="E59">
         <v>33.89984858106718</v>
       </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1511,6 +1806,11 @@
       <c r="E60">
         <v>37.50093065085732</v>
       </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1530,6 +1830,11 @@
       <c r="E61">
         <v>47.64297728475222</v>
       </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1549,6 +1854,11 @@
       <c r="E62">
         <v>36.90524015320087</v>
       </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1568,6 +1878,11 @@
       <c r="E63">
         <v>33.18744365555313</v>
       </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1587,6 +1902,11 @@
       <c r="E64">
         <v>45.40256176027109</v>
       </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -1606,6 +1926,11 @@
       <c r="E65">
         <v>42.67783065730858</v>
       </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -1625,6 +1950,11 @@
       <c r="E66">
         <v>51.2081347674178</v>
       </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1644,6 +1974,11 @@
       <c r="E67">
         <v>36.33516965859189</v>
       </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1663,6 +1998,11 @@
       <c r="E68">
         <v>22.82245652981953</v>
       </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1682,6 +2022,11 @@
       <c r="E69">
         <v>63.25493391093637</v>
       </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1701,6 +2046,11 @@
       <c r="E70">
         <v>42.47640237326462</v>
       </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -1720,6 +2070,11 @@
       <c r="E71">
         <v>38.86562533105315</v>
       </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -1739,6 +2094,11 @@
       <c r="E72">
         <v>39.05384664488866</v>
       </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -1758,6 +2118,11 @@
       <c r="E73">
         <v>35.48188509091392</v>
       </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -1777,6 +2142,11 @@
       <c r="E74">
         <v>40.67063274536932</v>
       </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -1796,6 +2166,11 @@
       <c r="E75">
         <v>41.01863287511839</v>
       </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -1815,6 +2190,11 @@
       <c r="E76">
         <v>38.26564347279876</v>
       </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -1834,6 +2214,11 @@
       <c r="E77">
         <v>31.47935403153563</v>
       </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -1853,6 +2238,11 @@
       <c r="E78">
         <v>33.24371567052008</v>
       </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -1872,6 +2262,11 @@
       <c r="E79">
         <v>24.25373579412955</v>
       </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -1891,6 +2286,11 @@
       <c r="E80">
         <v>37.35033916115638</v>
       </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -1910,6 +2310,11 @@
       <c r="E81">
         <v>29.37336716659092</v>
       </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -1929,6 +2334,11 @@
       <c r="E82">
         <v>30.10527064049046</v>
       </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -1948,6 +2358,11 @@
       <c r="E83">
         <v>34.22584013771567</v>
       </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -1967,6 +2382,11 @@
       <c r="E84">
         <v>35.64992477141099</v>
       </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -1986,6 +2406,11 @@
       <c r="E85">
         <v>32.01607560188073</v>
       </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -2005,6 +2430,11 @@
       <c r="E86">
         <v>35.2531643559153</v>
       </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -2024,6 +2454,11 @@
       <c r="E87">
         <v>37.91665284822803</v>
       </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -2043,6 +2478,11 @@
       <c r="E88">
         <v>29.95371835816143</v>
       </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -2062,6 +2502,11 @@
       <c r="E89">
         <v>48.07692563831609</v>
       </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -2081,6 +2526,11 @@
       <c r="E90">
         <v>33.81362816645177</v>
       </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -2100,6 +2550,11 @@
       <c r="E91">
         <v>39.77692615714009</v>
       </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -2119,6 +2574,11 @@
       <c r="E92">
         <v>40.45249611384582</v>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -2138,6 +2598,11 @@
       <c r="E93">
         <v>58.55960847320218</v>
       </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -2157,6 +2622,11 @@
       <c r="E94">
         <v>41.40086578889306</v>
       </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -2176,6 +2646,11 @@
       <c r="E95">
         <v>36.84217991374702</v>
       </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -2195,6 +2670,11 @@
       <c r="E96">
         <v>53.58060789650659</v>
       </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -2214,6 +2694,11 @@
       <c r="E97">
         <v>29.74025095783723</v>
       </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -2233,6 +2718,11 @@
       <c r="E98">
         <v>33.03048498260687</v>
       </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -2252,6 +2742,11 @@
       <c r="E99">
         <v>35.28617358120925</v>
       </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -2271,6 +2766,11 @@
       <c r="E100">
         <v>35.73961533910233</v>
       </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -2289,6 +2789,11 @@
       </c>
       <c r="E101">
         <v>38.78756319725969</v>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>